<commit_message>
Adding the Grading Sheet
</commit_message>
<xml_diff>
--- a/CSci130_Project_gradingsheet.xlsx
+++ b/CSci130_Project_gradingsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\Desktop\Stuff\School\Classes\CSCI 130 - Web Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\CSCI_130_Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -878,7 +878,7 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -892,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -906,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="D42">
         <f>SUM(D3:D40)</f>
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>